<commit_message>
Update 1018 7 PM
</commit_message>
<xml_diff>
--- a/Data/GGEE_23_Locations_2.xlsx
+++ b/Data/GGEE_23_Locations_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristachisholm/Documents/GitHub/GGEESummer23/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristadulany/Documents/GitHub/GGEESummer23/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2593D824-6872-694F-93B4-8D926446C0CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C39B72-9583-264C-B4EC-C8CED89CBEA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="740" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1160" yWindow="740" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
     <t>District</t>
   </si>
   <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>Brevard County</t>
   </si>
   <si>
@@ -66,6 +63,9 @@
   </si>
   <si>
     <t>Number of Programs</t>
+  </si>
+  <si>
+    <t>Number of Students</t>
   </si>
 </sst>
 </file>
@@ -421,7 +421,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -435,15 +435,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>20</v>
@@ -454,7 +454,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>23</v>
@@ -465,7 +465,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>90</v>
@@ -476,7 +476,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>90</v>
@@ -487,7 +487,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <f>62+26</f>
@@ -499,7 +499,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>40</v>
@@ -510,7 +510,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>336</v>
@@ -521,7 +521,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>26</v>

</xml_diff>